<commit_message>
Scripting SCD0204 - Validasi Mockup Digisales Mobile and SCD0205 - Validasi Field report PHR pada searching portal
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0178 - Validasi Mockup Portal.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0178 - Validasi Mockup Portal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C64D22F-6518-4FF9-B70A-304C0031A496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7937A6-72AD-42B2-A45F-33A94B114939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>ReportProductHolding.xlsx</t>
+  </si>
+  <si>
+    <t>TEXT4</t>
+  </si>
+  <si>
+    <t>TEXT5</t>
   </si>
 </sst>
 </file>
@@ -501,7 +507,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,9 +525,8 @@
     <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -570,6 +575,12 @@
         <v>21</v>
       </c>
       <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -612,11 +623,10 @@
       <c r="N2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="8"/>
+      <c r="Q2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8"/>
     </row>

</xml_diff>